<commit_message>
Drobne zmiany i skorygowane ikonki
</commit_message>
<xml_diff>
--- a/Schemat ikonek w alfanumerycznym.xlsx
+++ b/Schemat ikonek w alfanumerycznym.xlsx
@@ -17,10 +17,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Czcionka tekstu podstawowego"/>
       <family val="2"/>
       <charset val="238"/>
@@ -181,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -190,14 +197,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -492,324 +502,464 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+      <selection activeCell="AH11" sqref="AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="31" width="2.375" customWidth="1"/>
+    <col min="1" max="32" width="2.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+    <row r="1" spans="1:32">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="1"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="9"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+    </row>
+    <row r="4" spans="1:32">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="1"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="1"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="9"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="2"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="9"/>
       <c r="S5" s="2"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="1"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+    </row>
+    <row r="6" spans="1:32">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" ht="15" thickBot="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="11"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" thickTop="1">
+      <c r="O6" s="2"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+    </row>
+    <row r="7" spans="1:32" ht="15" thickBot="1">
+      <c r="A7" s="10"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+    </row>
+    <row r="8" spans="1:32" ht="15" thickTop="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="8"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
       <c r="N8" s="7"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
       <c r="U8" s="7"/>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+    </row>
+    <row r="9" spans="1:32">
+      <c r="A9" s="2"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="2"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+    </row>
+    <row r="10" spans="1:32">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="1"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+    </row>
+    <row r="11" spans="1:32">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="1"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="1"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="9"/>
       <c r="S11" s="2"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+    </row>
+    <row r="12" spans="1:32">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+    </row>
+    <row r="14" spans="1:32">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
     </row>
     <row r="17" spans="1:31">
       <c r="A17" s="1"/>
@@ -825,7 +975,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="1"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="15"/>
+      <c r="N17" s="9"/>
       <c r="O17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -839,8 +989,8 @@
       <c r="Z17" s="6"/>
       <c r="AA17" s="4"/>
       <c r="AB17" s="1"/>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="15"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
       <c r="AE17" s="1"/>
     </row>
     <row r="18" spans="1:31">
@@ -870,10 +1020,10 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="5"/>
       <c r="AA18" s="4"/>
-      <c r="AB18" s="15"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
     </row>
     <row r="19" spans="1:31">
       <c r="A19" s="1"/>
@@ -904,12 +1054,12 @@
       <c r="AA19" s="3"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="2"/>
+      <c r="AD19" s="9"/>
       <c r="AE19" s="1"/>
     </row>
     <row r="20" spans="1:31">
       <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="6"/>

</xml_diff>